<commit_message>
Little fixes to mq136
</commit_message>
<xml_diff>
--- a/WPDigitalizer/MQ136/MQ 136 análisis.xlsx
+++ b/WPDigitalizer/MQ136/MQ 136 análisis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c88fdd8443585846/Escritorio/MQSensorsLib_Docs/WPDigitalizer/MQ136/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\OneDrive\Escritorio\MQSensorsLib_Docs\WPDigitalizer\MQ136\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D7E184CA-18BF-47F7-A09B-8FDCAB1B486C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7BE488-EC4E-42F6-8C91-634244A49DD2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A283E8-EC4E-454C-A3D3-D3DD492CA5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E7386C9A-BD4F-4764-9504-B933BB372B25}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E7386C9A-BD4F-4764-9504-B933BB372B25}"/>
   </bookViews>
   <sheets>
     <sheet name="H2S" sheetId="1" r:id="rId1"/>
@@ -275,6 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,7 +300,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +446,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -884,7 +884,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1322,7 +1322,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1750,6 +1750,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>AIR!$A$3:$A$14</c:f>
@@ -4723,7 +4737,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4738,10 +4752,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -4916,8 +4930,13 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1">
+        <f>(1043.3)*((A19)^-3.282)</f>
+        <v>2.9141828874885021</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -4962,16 +4981,16 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -5098,17 +5117,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8634364C-4473-41C2-884D-F64703EA4435}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -5122,7 +5141,7 @@
       <c r="A3" s="3">
         <v>2.8507869769701601</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="14">
         <v>9.8665605346682597</v>
       </c>
     </row>
@@ -5130,7 +5149,7 @@
       <c r="A4" s="4">
         <v>2.5206802855550801</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="14">
         <v>15.8957280955174</v>
       </c>
     </row>
@@ -5138,7 +5157,7 @@
       <c r="A5" s="8">
         <v>2.3946068399985601</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="14">
         <v>19.575405239772799</v>
       </c>
     </row>
@@ -5146,7 +5165,7 @@
       <c r="A6" s="8">
         <v>2.2293547152559001</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="14">
         <v>23.785204084464802</v>
       </c>
     </row>
@@ -5154,7 +5173,7 @@
       <c r="A7" s="8">
         <v>2.13968758658506</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="14">
         <v>28.1342001330577</v>
       </c>
     </row>
@@ -5162,7 +5181,7 @@
       <c r="A8" s="8">
         <v>1.99175625546632</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="14">
         <v>35.590438509021801</v>
       </c>
     </row>
@@ -5170,7 +5189,7 @@
       <c r="A9" s="8">
         <v>1.9111684619631399</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="14">
         <v>45.326189803283199</v>
       </c>
     </row>
@@ -5178,7 +5197,7 @@
       <c r="A10" s="8">
         <v>1.7615206736740501</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="14">
         <v>53.613838698463397</v>
       </c>
     </row>
@@ -5186,7 +5205,7 @@
       <c r="A11" s="8">
         <v>1.6733791092486401</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="14">
         <v>66.469796173740605</v>
       </c>
     </row>
@@ -5194,7 +5213,7 @@
       <c r="A12" s="8">
         <v>1.54105613788171</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="14">
         <v>100.805683599557</v>
       </c>
     </row>
@@ -5202,7 +5221,7 @@
       <c r="A13" s="8">
         <v>1.43434955888966</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="14">
         <v>131.87708033960999</v>
       </c>
     </row>
@@ -5210,7 +5229,7 @@
       <c r="A14" s="10">
         <v>1.3764085170002101</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="14">
         <v>164.60153270291499</v>
       </c>
     </row>
@@ -5234,17 +5253,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC87F5F-D26C-44D9-A361-9BC89CBDF81C}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">

</xml_diff>